<commit_message>
--- title: 'pyKP项目进度日志' author: '黄炎' date: '2020-10-16' ---
# 项目进度

### 1015
- cluster 完成
- improved autocomplete performance

### 1013
- layer完成
</commit_message>
<xml_diff>
--- a/cluster_test.xlsx
+++ b/cluster_test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Site</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>official_cluster_4</t>
+  </si>
+  <si>
+    <t>official_cluster_311111111111111111111111111111111111111111</t>
   </si>
 </sst>
 </file>
@@ -362,7 +365,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -377,7 +380,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>15321</v>

</xml_diff>